<commit_message>
Added tests for NumStrDto Method ShiftPrecisionRight
</commit_message>
<xml_diff>
--- a/notes/Notes.xlsx
+++ b/notes/Notes.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\go\work\src\MikeAustin71\mathopsgo\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57F2064-E681-48CE-92D3-D33B0CC11CE6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F744C71-ED6A-4A5F-9C53-33252CA8DD8A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21555" windowHeight="7980" xr2:uid="{52560440-40DB-49E3-B993-D505A6A0DDF8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21555" windowHeight="7980" activeTab="1" xr2:uid="{52560440-40DB-49E3-B993-D505A6A0DDF8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="ShiftPrecisionLeft" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
   <si>
     <t>Precision</t>
   </si>
@@ -72,12 +73,21 @@
   </si>
   <si>
     <t>0.000</t>
+  </si>
+  <si>
+    <t>Shift Precision Right</t>
+  </si>
+  <si>
+    <t>Shift Relative Decimal Position Right X-Number of places</t>
+  </si>
+  <si>
+    <t>NumStrDto.ShiftPrecisionRight()-----&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,20 +225,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -246,9 +250,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -256,13 +257,51 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{EF1C1AFE-7348-4D28-8347-E37773B4EA63}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -573,131 +612,131 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9511E72-D9F3-4D48-8BC1-0698570F0819}">
   <dimension ref="B1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="30" x14ac:dyDescent="0.4">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="11"/>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="11"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="2:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>123456.789</v>
       </c>
-      <c r="C7" s="10">
-        <v>3</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7">
         <v>123.456789</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>123456.789</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>2</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="7">
         <v>1234.56789</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>123456.789</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <v>6</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>0.123456789</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>123456789</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="8">
         <v>6</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="7">
         <v>123.456789</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>123</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="8">
         <v>5</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="7">
         <v>1.23E-3</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>0</v>
       </c>
-      <c r="C12" s="10">
-        <v>3</v>
-      </c>
-      <c r="D12" s="17" t="s">
+      <c r="C12" s="8">
+        <v>3</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <v>-123456.789</v>
       </c>
-      <c r="C13" s="10">
-        <v>3</v>
-      </c>
-      <c r="D13" s="9">
+      <c r="C13" s="8">
+        <v>3</v>
+      </c>
+      <c r="D13" s="7">
         <v>-123.456789</v>
       </c>
     </row>
@@ -710,6 +749,158 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730415AE-1F09-4858-9A9C-FDE1F55EA077}">
+  <dimension ref="B1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="22.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="30" x14ac:dyDescent="0.4">
+      <c r="B1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="2:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>123456.789</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>123456.789</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7">
+        <v>12345678.9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="7">
+        <v>123456.789</v>
+      </c>
+      <c r="C9" s="8">
+        <v>6</v>
+      </c>
+      <c r="D9" s="18">
+        <v>123456789000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
+        <v>123456789</v>
+      </c>
+      <c r="C10" s="8">
+        <v>6</v>
+      </c>
+      <c r="D10" s="18">
+        <v>123456789000000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
+        <v>123</v>
+      </c>
+      <c r="C11" s="8">
+        <v>5</v>
+      </c>
+      <c r="D11" s="7">
+        <v>12300000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>3</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="7">
+        <v>123456.789</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0</v>
+      </c>
+      <c r="D13" s="14">
+        <v>123456.789</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="7">
+        <v>-123456.789</v>
+      </c>
+      <c r="C14" s="8">
+        <v>3</v>
+      </c>
+      <c r="D14" s="7">
+        <v>-123.456789</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2BC69A-7F8A-4E1E-BF48-086C3E46508D}">
   <dimension ref="B1:AB7"/>
   <sheetViews>
@@ -726,77 +917,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="1" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
     </row>
     <row r="2" spans="2:28" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E2" s="7">
+      <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <v>2</v>
       </c>
-      <c r="G2" s="7">
-        <v>3</v>
-      </c>
-      <c r="H2" s="7">
+      <c r="G2" s="5">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5">
         <v>4</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="5">
         <v>5</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="5">
         <v>6</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="5">
         <v>7</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="7">
+      <c r="M2" s="2"/>
+      <c r="N2" s="5">
         <v>1</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="5">
         <v>2</v>
       </c>
-      <c r="P2" s="7">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="8" t="s">
+      <c r="P2" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="7">
+      <c r="R2" s="5">
         <v>4</v>
       </c>
-      <c r="S2" s="7">
+      <c r="S2" s="5">
         <v>5</v>
       </c>
-      <c r="T2" s="7">
+      <c r="T2" s="5">
         <v>6</v>
       </c>
-      <c r="U2" s="7">
+      <c r="U2" s="5">
         <v>7</v>
       </c>
     </row>
@@ -807,7 +998,7 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="M3" s="3"/>
+      <c r="M3" s="2"/>
       <c r="AA3" t="s">
         <v>0</v>
       </c>
@@ -822,7 +1013,7 @@
       <c r="C4">
         <v>7</v>
       </c>
-      <c r="M4" s="3"/>
+      <c r="M4" s="2"/>
       <c r="AA4" t="s">
         <v>1</v>
       </c>
@@ -837,7 +1028,7 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="M5" s="3"/>
+      <c r="M5" s="2"/>
       <c r="AA5" t="s">
         <v>2</v>
       </c>
@@ -860,29 +1051,29 @@
       </c>
     </row>
     <row r="7" spans="2:28" ht="21" x14ac:dyDescent="0.35">
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -895,7 +1086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{189A2D4A-648C-4F72-94C6-DD68E40F40C4}">
   <dimension ref="B1:W5"/>
   <sheetViews>
@@ -912,26 +1103,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="1" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
     </row>
     <row r="2" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
@@ -961,7 +1152,7 @@
       <c r="K2">
         <v>7</v>
       </c>
-      <c r="L2" s="3"/>
+      <c r="L2" s="2"/>
       <c r="M2">
         <v>1</v>
       </c>
@@ -971,7 +1162,7 @@
       <c r="O2">
         <v>3</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="Q2">
@@ -1000,7 +1191,7 @@
       <c r="C3">
         <v>7</v>
       </c>
-      <c r="L3" s="3"/>
+      <c r="L3" s="2"/>
       <c r="V3" t="s">
         <v>1</v>
       </c>
@@ -1015,7 +1206,7 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="2"/>
       <c r="V4" t="s">
         <v>2</v>
       </c>
@@ -1030,7 +1221,7 @@
       <c r="C5">
         <v>7</v>
       </c>
-      <c r="L5" s="3"/>
+      <c r="L5" s="2"/>
       <c r="V5" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Updated Notes Excel Spreadsheet
</commit_message>
<xml_diff>
--- a/notes/Notes.xlsx
+++ b/notes/Notes.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\go\work\src\MikeAustin71\mathopsgo\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F744C71-ED6A-4A5F-9C53-33252CA8DD8A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F235E4-D107-4F12-A1DE-E0C147678FDC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21555" windowHeight="7980" activeTab="1" xr2:uid="{52560440-40DB-49E3-B993-D505A6A0DDF8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21555" windowHeight="7980" xr2:uid="{52560440-40DB-49E3-B993-D505A6A0DDF8}"/>
   </bookViews>
   <sheets>
     <sheet name="ShiftPrecisionLeft" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId2"/>
+    <sheet name="ShiftPrecisionRight" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>Precision</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>NumStrDto.ShiftPrecisionRight()-----&gt;</t>
+  </si>
+  <si>
+    <t>0.00000</t>
+  </si>
+  <si>
+    <t>-123456789000000</t>
   </si>
 </sst>
 </file>
@@ -610,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9511E72-D9F3-4D48-8BC1-0698570F0819}">
-  <dimension ref="B1:D13"/>
+  <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" x14ac:dyDescent="0.3"/>
@@ -730,13 +736,57 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="7">
+      <c r="B13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="8">
+        <v>2</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="14">
+        <v>123456.789</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="14">
+        <v>123456.789</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="14">
         <v>-123456.789</v>
       </c>
-      <c r="C13" s="8">
-        <v>3</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="14">
+        <v>-123456.789</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="7">
+        <v>-123456.789</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7">
+        <v>-123.456789</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="7">
+        <v>-123456789</v>
+      </c>
+      <c r="C17" s="8">
+        <v>6</v>
+      </c>
+      <c r="D17" s="7">
         <v>-123.456789</v>
       </c>
     </row>
@@ -750,10 +800,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730415AE-1F09-4858-9A9C-FDE1F55EA077}">
-  <dimension ref="B1:D14"/>
+  <dimension ref="B1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" x14ac:dyDescent="0.3"/>
@@ -885,10 +935,32 @@
         <v>-123456.789</v>
       </c>
       <c r="C14" s="8">
-        <v>3</v>
-      </c>
-      <c r="D14" s="7">
-        <v>-123.456789</v>
+        <v>0</v>
+      </c>
+      <c r="D14" s="14">
+        <v>-123456.789</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="7">
+        <v>-123456.789</v>
+      </c>
+      <c r="C15" s="8">
+        <v>3</v>
+      </c>
+      <c r="D15" s="7">
+        <v>-123456789</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="7">
+        <v>-123456789</v>
+      </c>
+      <c r="C16" s="8">
+        <v>6</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added nth root notes.
</commit_message>
<xml_diff>
--- a/notes/Notes.xlsx
+++ b/notes/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\go\work\src\MikeAustin71\mathopsgo\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F4F112-3224-4124-A0BD-D205C4AA51B0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84B8C78-19C0-4780-B2ED-0F072D60163C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21555" windowHeight="7980" activeTab="4" xr2:uid="{52560440-40DB-49E3-B993-D505A6A0DDF8}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Precision</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>Digits</t>
+  </si>
+  <si>
+    <t>Power=</t>
+  </si>
+  <si>
+    <t>Number of digits = scaleVal Power + 1</t>
   </si>
 </sst>
 </file>
@@ -1320,25 +1326,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122D42F9-87B9-4EE2-98D7-C014FAFE289D}">
-  <dimension ref="H4:U8"/>
+  <dimension ref="G4:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:21" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:21" x14ac:dyDescent="0.25">
       <c r="I6">
         <v>57.625</v>
       </c>
     </row>
-    <row r="7" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="7:21" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
         <v>21</v>
       </c>
@@ -1382,7 +1388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:21" x14ac:dyDescent="0.25">
       <c r="I8">
         <v>5</v>
       </c>
@@ -1421,6 +1427,27 @@
       </c>
       <c r="U8">
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="7:21" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>57.859000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="7:21" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>